<commit_message>
Updates following earlier call
</commit_message>
<xml_diff>
--- a/test/resources/Supplier Test Cases/GP system test cases - REQUESTS.xlsx
+++ b/test/resources/Supplier Test Cases/GP system test cases - REQUESTS.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="18930" windowHeight="7665" tabRatio="861" firstSheet="4" activeTab="11"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="18930" windowHeight="7665" tabRatio="861" firstSheet="2" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Index GP requests" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="92">
   <si>
     <t>Test Case</t>
   </si>
@@ -677,53 +677,6 @@
     <t xml:space="preserve">A GP system must be able to send a test request in FHIR format for a 'FBC' + 'Urine' test  </t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">A </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>test request</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> message for a </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Profile\Panel test (Blood - full blood count, electrolytes and creatinine, cholesterol and triglycerides, glycated haemoglobin , Urine - urine albumin  ) </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> has been CREATED within the GP system (In line with the spec: https://developer.nhs.uk/apis/itk3nationalpathology-1-1-0/index.html)</t>
-    </r>
-  </si>
-  <si>
     <t>Test Case Ref:</t>
   </si>
   <si>
@@ -818,15 +771,6 @@
     <t>The request message is sent to LIMS (via order comms if applicabl;e)</t>
   </si>
   <si>
-    <t>GP sending a 'Pathology Request' FHIR message with status of 'interim' for a profile/panel test ("Prostate Antigen Test")  to LIMs</t>
-  </si>
-  <si>
-    <t>GP sending a 'Pathology Request' FHIR message with status of 'Uknown' for a profile\panel test ("Prostate Antigen Test") to LIMS</t>
-  </si>
-  <si>
-    <t>GP Sending a 'Pathology Reuest' FHIR message with status of 'Final' for a profile\panel test ("Prostate Antigen Test")to LIMS</t>
-  </si>
-  <si>
     <t>This test is to check for messaging contains status of 'Uknown'</t>
   </si>
   <si>
@@ -856,6 +800,221 @@
   <si>
     <t xml:space="preserve">* Requires a valid  test request for a "Prostate Specific Antigen" from a GP system in the correct FHIR message format
 </t>
+  </si>
+  <si>
+    <r>
+      <t>A valid UTL code "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1107811000000102</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" is present within the request message</t>
+    </r>
+  </si>
+  <si>
+    <t>Valid UTL codes are present within the request message, as per below:
+1107871000000107 Sodium substance concentration in serum
+1107761000000109 Potassium substance concentration in serum
+"1106511000000102 " Chloride substance concentration in serum
+1107001000000108 Creatinine substance concentration in serum
+1107411000000104 Estimated glomerular filtration rate by laboratory calculation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GP sending a 'Pathology Request' FHIR message  for a standalone ("Prostate Antigen Test")  to LIMs. (This request is a  pre-req to running LIMS_1.1.9 (which tests  'partial' status of a result) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GP sending a 'Pathology Request' FHIR message  for a standalone ("Prostate Antigen Test")  to LIMs. (This request is a  pre-req to running LIMS_1.1.9 (which tests  'Uknown' status of a result) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GP sending a 'Pathology Request' FHIR message  for a standalone ("Prostate Antigen Test")  to LIMs. (This request is a  pre-req to running LIMS_1.1.9 (which tests  'Final' status of a result) </t>
+  </si>
+  <si>
+    <r>
+      <t>A valid UTL code "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+1107871000000107 Sodium substance concentration in serum
+1107761000000109 Potassium substance concentration in serum
+"1106511000000102 " Chloride substance concentration in serum
+1107001000000108 Creatinine substance concentration in serum
+1107411000000104 Estimated glomerular filtration rate by laboratory calculation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" is present within the request message</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>test request</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> message for both a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Profile\Panel test (Blood - full blood count, electrolytes and creatinine, cholesterol and triglycerides, glycated haemoglobin ) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>And</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (Urine - urine albumin ) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> has been CREATED within the GP system (In line with the spec: https://developer.nhs.uk/apis/itk3nationalpathology-1-1-0/index.html)</t>
+    </r>
+  </si>
+  <si>
+    <t>A valid UTL code '57371000237100' is present within the request message</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A valid UTL code is present withn the message:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>FBC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+1107511000000100 Haemoglobin mass concentration in blood
+1110441000000100 White blood cell count in blood
+1108041000000107 Platelet count in blood
+1111571000000101? Haematocrit volume fraction of blood?
+1022451000000103 Red blood cell count
+Not found Not found
+"1022471000000107  ?" MCH - Mean corpuscular haemoglobin?
+Not found Not found
+1108071000000101 Neutrophil count in blood
+67541000237108 Lymphocyte count in blood
+1107991000000100 Monocyte count in blood
+1107391000000104 Eosinophil count in blood
+1106091000000103 Basophil count in blood
+58571000237106 Nucleated red blood cell count in blood
+"993501000000105 " Red blood cell distribution width
+993481000000101 Mean platelet volume
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Electrolytes &amp; Creatnine</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+1107871000000107 Sodium substance concentration in serum
+1107761000000109 Potassium substance concentration in serum
+1106511000000102 Chloride substance concentration in serum
+1107001000000108 Creatinine substance concentration in serum
+1107411000000104 Estimated glomerular filtration rate by laboratory calculation</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -3862,9 +4021,6 @@
     <xf numFmtId="0" fontId="34" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="34" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -3875,6 +4031,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -6414,8 +6573,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AI30"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="118" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView topLeftCell="A4" zoomScale="118" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6433,41 +6592,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
     </row>
     <row r="2" spans="1:35" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="56"/>
-      <c r="B2" s="56"/>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
+      <c r="A2" s="55"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
     </row>
     <row r="3" spans="1:35" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="57"/>
-      <c r="B3" s="57"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="57"/>
+      <c r="A3" s="56"/>
+      <c r="B3" s="56"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="56"/>
       <c r="G3" s="32"/>
     </row>
     <row r="4" spans="1:35" s="25" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A4" s="47" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B4" s="47" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="47" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D4" s="47" t="s">
         <v>1</v>
@@ -6512,13 +6671,13 @@
     </row>
     <row r="5" spans="1:35" s="40" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="37" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B5" s="43" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="52" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D5" s="37" t="s">
         <v>36</v>
@@ -6536,16 +6695,16 @@
     </row>
     <row r="6" spans="1:35" s="40" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="37" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B6" s="43" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="52" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D6" s="37" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E6" s="38" t="s">
         <v>19</v>
@@ -6560,13 +6719,13 @@
     </row>
     <row r="7" spans="1:35" s="40" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="37" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B7" s="43" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="52" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D7" s="37" t="s">
         <v>38</v>
@@ -6584,13 +6743,13 @@
     </row>
     <row r="8" spans="1:35" s="40" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="37" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B8" s="43" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="52" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D8" s="37" t="s">
         <v>39</v>
@@ -6606,87 +6765,87 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:35" s="26" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35" s="57" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="49" t="s">
-        <v>60</v>
-      </c>
-      <c r="B9" s="53" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" s="49" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="52" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D9" s="49" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="E9" s="50" t="s">
         <v>31</v>
       </c>
       <c r="F9" s="51" t="str">
         <f t="shared" ref="F9:F11" si="3">(LEFT(A9,3)&amp;". "&amp;D9)</f>
-        <v>GP_. GP sending a 'Pathology Request' FHIR message with status of 'interim' for a profile/panel test ("Prostate Antigen Test")  to LIMs</v>
+        <v xml:space="preserve">GP_. GP sending a 'Pathology Request' FHIR message  for a standalone ("Prostate Antigen Test")  to LIMs. (This request is a  pre-req to running LIMS_1.1.9 (which tests  'partial' status of a result) </v>
       </c>
       <c r="G9" s="39" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:35" s="57" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="49" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" s="49" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="52" t="s">
+        <v>77</v>
+      </c>
+      <c r="D10" s="49" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="10" spans="1:35" s="26" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="49" t="s">
-        <v>61</v>
-      </c>
-      <c r="B10" s="53" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="52" t="s">
-        <v>81</v>
-      </c>
-      <c r="D10" s="49" t="s">
-        <v>76</v>
-      </c>
       <c r="E10" s="50" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F10" s="51" t="str">
         <f t="shared" si="3"/>
-        <v>GP_. GP sending a 'Pathology Request' FHIR message with status of 'Uknown' for a profile\panel test ("Prostate Antigen Test") to LIMS</v>
+        <v xml:space="preserve">GP_. GP sending a 'Pathology Request' FHIR message  for a standalone ("Prostate Antigen Test")  to LIMs. (This request is a  pre-req to running LIMS_1.1.9 (which tests  'Uknown' status of a result) </v>
       </c>
       <c r="G10" s="39" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="11" spans="1:35" s="26" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:35" s="57" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="49" t="s">
-        <v>62</v>
-      </c>
-      <c r="B11" s="53" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" s="49" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="52" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D11" s="49" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="E11" s="50" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F11" s="51" t="str">
         <f t="shared" si="3"/>
-        <v>GP_. GP Sending a 'Pathology Reuest' FHIR message with status of 'Final' for a profile\panel test ("Prostate Antigen Test")to LIMS</v>
+        <v xml:space="preserve">GP_. GP sending a 'Pathology Request' FHIR message  for a standalone ("Prostate Antigen Test")  to LIMs. (This request is a  pre-req to running LIMS_1.1.9 (which tests  'Final' status of a result) </v>
       </c>
       <c r="G11" s="39" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:35" s="40" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="37" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B12" s="43" t="s">
         <v>13</v>
       </c>
       <c r="C12" s="52" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D12" s="37" t="s">
         <v>42</v>
@@ -6705,13 +6864,13 @@
     </row>
     <row r="13" spans="1:35" s="40" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="37" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B13" s="43" t="s">
         <v>14</v>
       </c>
       <c r="C13" s="52" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D13" s="37" t="s">
         <v>44</v>
@@ -6730,13 +6889,13 @@
     </row>
     <row r="14" spans="1:35" s="40" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="37" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B14" s="43" t="s">
         <v>20</v>
       </c>
       <c r="C14" s="52" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D14" s="37" t="s">
         <v>51</v>
@@ -6755,13 +6914,13 @@
     </row>
     <row r="15" spans="1:35" s="46" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="37" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B15" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="54" t="s">
-        <v>84</v>
+      <c r="C15" s="53" t="s">
+        <v>80</v>
       </c>
       <c r="D15" s="44" t="s">
         <v>52</v>
@@ -6908,10 +7067,10 @@
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet10"/>
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6978,7 +7137,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C6" s="35"/>
       <c r="E6" s="23"/>
@@ -6988,7 +7147,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C7" s="35"/>
       <c r="D7" s="11"/>
@@ -7003,30 +7162,35 @@
       <c r="C8" s="35"/>
       <c r="D8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="C9"/>
+    <row r="9" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C9" s="35"/>
       <c r="D9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="C10"/>
-      <c r="D10" s="11"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-    </row>
-    <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12"/>
-      <c r="B12" s="36"/>
-      <c r="D12" s="1" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11"/>
+      <c r="B11" s="36"/>
+      <c r="D11" s="1" t="s">
         <v>8</v>
       </c>
     </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D12"/>
+    </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="9"/>
+      <c r="C13"/>
       <c r="D13"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -7041,8 +7205,6 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" s="9"/>
-      <c r="C16"/>
-      <c r="D16"/>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="9"/>
@@ -7061,24 +7223,21 @@
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" s="9"/>
+      <c r="C22" s="6"/>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" s="9"/>
-      <c r="C23" s="6"/>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" s="9"/>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B25" s="9"/>
+      <c r="C25" s="10"/>
     </row>
     <row r="26" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B26" s="9"/>
       <c r="C26" s="10"/>
-    </row>
-    <row r="27" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B27" s="9"/>
-      <c r="C27" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7088,10 +7247,10 @@
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet11"/>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7161,7 +7320,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C6" s="35"/>
       <c r="E6" s="23"/>
@@ -7171,7 +7330,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C7" s="35"/>
       <c r="D7" s="11"/>
@@ -7187,29 +7346,34 @@
       <c r="D8" s="11"/>
     </row>
     <row r="9" spans="1:5" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
+      <c r="A9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>90</v>
+      </c>
       <c r="C9"/>
       <c r="D9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="C10"/>
-      <c r="D10" s="11"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-    </row>
-    <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12"/>
-      <c r="B12" s="36"/>
-      <c r="D12" s="1" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11"/>
+      <c r="B11" s="36"/>
+      <c r="D11" s="1" t="s">
         <v>8</v>
       </c>
     </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D12"/>
+    </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="9"/>
+      <c r="C13"/>
       <c r="D13"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -7219,29 +7383,24 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" s="9"/>
-      <c r="C15"/>
-      <c r="D15"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" s="9"/>
+      <c r="C16" s="6"/>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="9"/>
-      <c r="C17" s="6"/>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="9"/>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B19" s="9"/>
+      <c r="C19" s="10"/>
     </row>
     <row r="20" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="9"/>
       <c r="C20" s="10"/>
-    </row>
-    <row r="21" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="9"/>
-      <c r="C21" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -7257,7 +7416,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7316,7 +7475,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>54</v>
+        <v>89</v>
       </c>
       <c r="C5" s="35"/>
       <c r="E5" s="17"/>
@@ -7326,7 +7485,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C6" s="35"/>
       <c r="E6" s="23"/>
@@ -7336,7 +7495,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C7" s="35"/>
       <c r="D7" s="11"/>
@@ -7351,8 +7510,13 @@
       <c r="C8" s="35"/>
       <c r="D8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
+    <row r="9" spans="1:5" ht="375" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>91</v>
+      </c>
       <c r="C9"/>
       <c r="D9" s="11"/>
     </row>
@@ -7418,16 +7582,17 @@
     <hyperlink ref="E2" location="'Index-Phase 1-LIMS-Test_List'!A1" display="Return to Index"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7463,7 +7628,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C3" s="33"/>
       <c r="E3" s="23"/>
@@ -7493,7 +7658,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C6" s="35"/>
       <c r="E6" s="23"/>
@@ -7503,7 +7668,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C7" s="35"/>
       <c r="D7" s="11"/>
@@ -7518,24 +7683,30 @@
       <c r="C8" s="35"/>
       <c r="D8" s="11"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-    </row>
-    <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10"/>
-      <c r="B10" s="36"/>
-      <c r="D10" s="1" t="s">
+    <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" s="35"/>
+      <c r="D9" s="11"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11"/>
+      <c r="B11" s="36"/>
+      <c r="D11" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D11"/>
-    </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="9"/>
       <c r="D12"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -7552,24 +7723,25 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" s="9"/>
-      <c r="C16" s="6"/>
+      <c r="D16"/>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="9"/>
+      <c r="C17" s="6"/>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="9"/>
     </row>
-    <row r="19" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="9"/>
-      <c r="C19" s="10"/>
     </row>
     <row r="20" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="9"/>
       <c r="C20" s="10"/>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B21" s="9"/>
+      <c r="C21" s="10"/>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" s="9"/>
@@ -7585,6 +7757,9 @@
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" s="9"/>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7595,10 +7770,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7664,7 +7839,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C6" s="35"/>
       <c r="E6" s="23"/>
@@ -7674,7 +7849,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C7" s="35"/>
       <c r="D7" s="11"/>
@@ -7689,24 +7864,30 @@
       <c r="C8" s="35"/>
       <c r="D8" s="11"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-    </row>
-    <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10"/>
-      <c r="B10" s="36"/>
-      <c r="D10" s="1" t="s">
+    <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" s="35"/>
+      <c r="D9" s="11"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11"/>
+      <c r="B11" s="36"/>
+      <c r="D11" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D11"/>
-    </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="9"/>
       <c r="D12"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -7723,24 +7904,25 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" s="9"/>
-      <c r="C16" s="6"/>
+      <c r="D16"/>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="9"/>
+      <c r="C17" s="6"/>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="9"/>
     </row>
-    <row r="19" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="9"/>
-      <c r="C19" s="10"/>
     </row>
     <row r="20" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="9"/>
       <c r="C20" s="10"/>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B21" s="9"/>
+      <c r="C21" s="10"/>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" s="9"/>
@@ -7756,6 +7938,9 @@
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" s="9"/>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7766,10 +7951,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7817,7 +8002,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C4" s="35"/>
       <c r="E4" s="17"/>
@@ -7837,7 +8022,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C6" s="35"/>
       <c r="E6" s="23"/>
@@ -7847,7 +8032,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C7" s="35"/>
       <c r="D7" s="11"/>
@@ -7862,28 +8047,33 @@
       <c r="C8" s="35"/>
       <c r="D8" s="11"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-    </row>
-    <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10"/>
-      <c r="B10"/>
-      <c r="C10" s="1" t="s">
+    <row r="9" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C9" s="35"/>
+      <c r="D9" s="11"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11"/>
+      <c r="B11"/>
+      <c r="C11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C11"/>
-      <c r="D11"/>
-    </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="9"/>
       <c r="C12"/>
       <c r="D12"/>
     </row>
@@ -7904,6 +8094,8 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" s="9"/>
+      <c r="C16"/>
+      <c r="D16"/>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="9"/>
@@ -7922,21 +8114,24 @@
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" s="9"/>
-      <c r="C22" s="6"/>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" s="9"/>
+      <c r="C23" s="6"/>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" s="9"/>
     </row>
-    <row r="25" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" s="9"/>
-      <c r="C25" s="10"/>
     </row>
     <row r="26" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B26" s="9"/>
       <c r="C26" s="10"/>
+    </row>
+    <row r="27" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B27" s="9"/>
+      <c r="C27" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -7950,10 +8145,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8021,7 +8216,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C6" s="35"/>
       <c r="E6" s="23"/>
@@ -8031,7 +8226,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C7" s="35"/>
       <c r="D7" s="11"/>
@@ -8046,28 +8241,33 @@
       <c r="C8" s="35"/>
       <c r="D8" s="11"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-    </row>
-    <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10"/>
-      <c r="B10"/>
-      <c r="C10" s="1" t="s">
+    <row r="9" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C9" s="35"/>
+      <c r="D9" s="11"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11"/>
+      <c r="B11"/>
+      <c r="C11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C11"/>
-      <c r="D11"/>
-    </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="9"/>
       <c r="C12"/>
       <c r="D12"/>
     </row>
@@ -8088,6 +8288,8 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" s="9"/>
+      <c r="C16"/>
+      <c r="D16"/>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="9"/>
@@ -8106,21 +8308,24 @@
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" s="9"/>
-      <c r="C22" s="6"/>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" s="9"/>
+      <c r="C23" s="6"/>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" s="9"/>
     </row>
-    <row r="25" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" s="9"/>
-      <c r="C25" s="10"/>
     </row>
     <row r="26" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B26" s="9"/>
       <c r="C26" s="10"/>
+    </row>
+    <row r="27" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B27" s="9"/>
+      <c r="C27" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -8134,10 +8339,10 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8156,7 +8361,7 @@
       </c>
       <c r="B1" s="7" t="str">
         <f ca="1">VLOOKUP(B2, 'Index GP requests'!A5:F65193,4, FALSE)</f>
-        <v>GP sending a 'Pathology Request' FHIR message with status of 'interim' for a profile/panel test ("Prostate Antigen Test")  to LIMs</v>
+        <v xml:space="preserve">GP sending a 'Pathology Request' FHIR message  for a standalone ("Prostate Antigen Test")  to LIMs. (This request is a  pre-req to running LIMS_1.1.9 (which tests  'partial' status of a result) </v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -8205,7 +8410,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C6" s="35"/>
       <c r="E6" s="23"/>
@@ -8215,7 +8420,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C7" s="35"/>
       <c r="D7" s="11"/>
@@ -8230,14 +8435,21 @@
       <c r="C8" s="35"/>
       <c r="D8" s="11"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
+    <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" s="35"/>
+      <c r="D9" s="11"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="9"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" s="9"/>
@@ -8253,21 +8465,24 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" s="9"/>
-      <c r="C15" s="6"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" s="9"/>
+      <c r="C16" s="6"/>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="9"/>
     </row>
-    <row r="18" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="9"/>
-      <c r="C18" s="10"/>
     </row>
     <row r="19" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B19" s="9"/>
       <c r="C19" s="10"/>
+    </row>
+    <row r="20" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B20" s="9"/>
+      <c r="C20" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -8281,10 +8496,10 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet7"/>
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8303,7 +8518,7 @@
       </c>
       <c r="B1" s="7" t="str">
         <f ca="1">VLOOKUP(B2, 'Index GP requests'!A5:F65193,4, FALSE)</f>
-        <v>GP sending a 'Pathology Request' FHIR message with status of 'Uknown' for a profile\panel test ("Prostate Antigen Test") to LIMS</v>
+        <v xml:space="preserve">GP sending a 'Pathology Request' FHIR message  for a standalone ("Prostate Antigen Test")  to LIMs. (This request is a  pre-req to running LIMS_1.1.9 (which tests  'Uknown' status of a result) </v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -8352,7 +8567,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C6" s="35"/>
       <c r="E6" s="23"/>
@@ -8362,7 +8577,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C7" s="35"/>
       <c r="D7" s="11"/>
@@ -8377,18 +8592,23 @@
       <c r="C8" s="35"/>
       <c r="D8" s="11"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
+    <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" s="35"/>
+      <c r="D9" s="11"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C10"/>
-      <c r="D10"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="9"/>
       <c r="C11"/>
       <c r="D11"/>
     </row>
@@ -8409,6 +8629,8 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" s="9"/>
+      <c r="C15"/>
+      <c r="D15"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" s="9"/>
@@ -8427,21 +8649,24 @@
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="9"/>
-      <c r="C21" s="6"/>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" s="9"/>
+      <c r="C22" s="6"/>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" s="9"/>
     </row>
-    <row r="24" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" s="9"/>
-      <c r="C24" s="10"/>
     </row>
     <row r="25" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B25" s="9"/>
       <c r="C25" s="10"/>
+    </row>
+    <row r="26" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B26" s="9"/>
+      <c r="C26" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -8454,10 +8679,10 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet8"/>
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8476,7 +8701,7 @@
       </c>
       <c r="B1" s="7" t="str">
         <f ca="1">VLOOKUP(B2, 'Index GP requests'!A5:F65193,4, FALSE)</f>
-        <v>GP Sending a 'Pathology Reuest' FHIR message with status of 'Final' for a profile\panel test ("Prostate Antigen Test")to LIMS</v>
+        <v xml:space="preserve">GP sending a 'Pathology Request' FHIR message  for a standalone ("Prostate Antigen Test")  to LIMs. (This request is a  pre-req to running LIMS_1.1.9 (which tests  'Final' status of a result) </v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -8525,7 +8750,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C6" s="35"/>
       <c r="E6" s="23"/>
@@ -8535,7 +8760,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C7" s="35"/>
       <c r="D7" s="11"/>
@@ -8550,33 +8775,43 @@
       <c r="C8" s="35"/>
       <c r="D8" s="11"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
+    <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" s="35"/>
+      <c r="D9" s="11"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="9"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" s="9"/>
-      <c r="C11" s="6"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" s="9"/>
+      <c r="C12" s="6"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" s="9"/>
     </row>
-    <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" s="9"/>
-      <c r="C14" s="10"/>
     </row>
     <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B15" s="9"/>
       <c r="C15" s="10"/>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B16" s="9"/>
+      <c r="C16" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -8592,7 +8827,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8659,7 +8894,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C6" s="35"/>
       <c r="E6" s="23"/>
@@ -8669,7 +8904,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C7" s="35"/>
       <c r="D7" s="11"/>
@@ -8684,9 +8919,14 @@
       <c r="C8" s="35"/>
       <c r="D8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="C9"/>
+    <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" s="35"/>
       <c r="D9" s="11"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>